<commit_message>
Update Authentification and change schript from Delay to Wait For..
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/Data_CSR_Management.xlsx
+++ b/Data Files/Website/DataFiles_CRM/Data_CSR_Management.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17930" windowHeight="6920"/>
+    <workbookView windowWidth="18530" windowHeight="7070"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <t>untuk registrasi</t>
   </si>
   <si>
-    <t>08974348089</t>
+    <t>0869815382</t>
   </si>
   <si>
     <t>Semua</t>
@@ -173,28 +173,28 @@
     <t>Nasabah Tidak Melanjutkan</t>
   </si>
   <si>
-    <t>+628974348089</t>
+    <t>+62869815382</t>
   </si>
   <si>
     <t>MIDGE001</t>
   </si>
   <si>
-    <t>sm34@yopmail.com</t>
-  </si>
-  <si>
-    <t>3171012805920001</t>
-  </si>
-  <si>
-    <t>M Angga Saputra</t>
+    <t>senyumku03618277@yopmail.com</t>
+  </si>
+  <si>
+    <t>3171014508770001</t>
+  </si>
+  <si>
+    <t>ANGGUN ZUMA RIANY</t>
   </si>
   <si>
     <t>JAKARTA</t>
   </si>
   <si>
-    <t>28/05/1992</t>
-  </si>
-  <si>
-    <t>LAKI-LAKI</t>
+    <t>05/08/1977</t>
+  </si>
+  <si>
+    <t>PEREMPUAN</t>
   </si>
   <si>
     <t>A</t>
@@ -313,10 +313,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -343,7 +343,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -351,6 +351,105 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,83 +464,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -454,29 +477,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -487,13 +487,109 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -505,43 +601,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,115 +655,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -684,8 +684,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -701,6 +716,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -754,42 +778,18 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -802,127 +802,127 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1262,8 +1262,8 @@
   <sheetPr/>
   <dimension ref="A1:AT3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2"/>
@@ -1277,7 +1277,7 @@
     <col min="7" max="7" width="24" customWidth="1"/>
     <col min="8" max="8" width="21.7272727272727" customWidth="1"/>
     <col min="9" max="10" width="13.7272727272727" customWidth="1"/>
-    <col min="11" max="11" width="28.4545454545455" customWidth="1"/>
+    <col min="11" max="11" width="35.2727272727273" customWidth="1"/>
     <col min="12" max="12" width="22.5454545454545" customWidth="1"/>
     <col min="13" max="13" width="16.4545454545455" customWidth="1"/>
     <col min="14" max="25" width="22.5454545454545" customWidth="1"/>
@@ -1588,35 +1588,29 @@
     </row>
   </sheetData>
   <dataValidations count="12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
+      <formula1>"Rekening Tabungan,Rekening Gaji,Transaksi Pribadi,Transaksi Bisnis,Lainnya"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:G2">
       <formula1>"Semua,Nasabah Baru,Nasabah Senyumku,Nasabah Tidak Melanjutkan"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
+      <formula1>"ACEH,BALI,BANTEN,BENGKULU,DAISTA YOGYAKARTA,DKI JAKARTA,JAMBI,JAWA BARAT,JAWA TENGAH,JAWA TIMUR,GORONTALO"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2">
+      <formula1>"KAB. ADM. KEP. SERIBU,KOTA ADM. JAKARTA PUSAT,KOTA ADM. JAKARTA UTARA,KOTA ADM. JAKARTA BARAT,KOTA ADM. JAKARTA SELATAN,KOTA ADM. JAKARTA TIMUR"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2">
       <formula1>"Tidak Sekolah,SD,SMP,SMA,Diploma,S1 (Sarjana),S2 (Magister),S3 (Doktoral),Profesor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2">
-      <formula1>"Jasa,Lainnya"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
-      <formula1>"ACEH,BALI,BANTEN,BENGKULU,DAISTA YOGYAKARTA,DKI JAKARTA,JAMBI,JAWA BARAT,JAWA TENGAH,JAWA TIMUR,GORONTALO"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2">
+      <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2">
       <formula1>"SETIA BUDI,TEBET,MAMPANG PRAPATAN,PASAR MINGGU,KEBAYORAN LAMA,CILANDAK,KEBAYORAN BARU,PANCORAN,JAGAKARSA,PESANGGRAHAN"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2">
-      <formula1>"KAB. ADM. KEP. SERIBU,KOTA ADM. JAKARTA PUSAT,KOTA ADM. JAKARTA UTARA,KOTA ADM. JAKARTA BARAT,KOTA ADM. JAKARTA SELATAN,KOTA ADM. JAKARTA TIMUR"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3">
-      <formula1>$AH$2:$AH$10</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2">
-      <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2">
       <formula1>"Katolik,Kristen,Islam,Budha,Hindu,Lainnya"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
-      <formula1>"Rekening Tabungan,Rekening Gaji,Transaksi Pribadi,Transaksi Bisnis,Lainnya"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Gaji Bulanan,Pemasukan dari Usaha,Hasil Investasi,Warisan,Danah Hibah,Dana Pinjaman,Hadiah,Pendapatan Jasa,Pendapatan dari Keluarga (Suami/Istri/Orang Tua)"</formula1>
@@ -1624,9 +1618,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2">
       <formula1>"Pegawai Swasta,Ibu Rumah Tangga,Lainnya"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2">
+      <formula1>"Jasa,Lainnya"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH3">
+      <formula1>$AH$2:$AH$10</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" display="sm34@yopmail.com" tooltip="mailto:sm34@yopmail.com"/>
+    <hyperlink ref="K2" r:id="rId1" display="senyumku03618277@yopmail.com" tooltip="mailto:senyumku03618277@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Update test suite and test data
</commit_message>
<xml_diff>
--- a/Data Files/Website/DataFiles_CRM/Data_CSR_Management.xlsx
+++ b/Data Files/Website/DataFiles_CRM/Data_CSR_Management.xlsx
@@ -158,7 +158,7 @@
     <t>untuk registrasi</t>
   </si>
   <si>
-    <t>+628183174101181</t>
+    <t>+62808958282</t>
   </si>
   <si>
     <t>Semua</t>
@@ -176,13 +176,13 @@
     <t>MIDGE001</t>
   </si>
   <si>
-    <t>stgcrmf320@yopmail.com</t>
-  </si>
-  <si>
-    <t>3171014202810001</t>
-  </si>
-  <si>
-    <t>YOANDA SYAHRINI</t>
+    <t>senyumku45622497@yopmail.com</t>
+  </si>
+  <si>
+    <t>3224035703880026</t>
+  </si>
+  <si>
+    <t>YEJI</t>
   </si>
   <si>
     <t>JAKARTA</t>
@@ -191,7 +191,7 @@
     <t>21/09/1990</t>
   </si>
   <si>
-    <t>LAKI-LAKI</t>
+    <t>PEREMPUAN</t>
   </si>
   <si>
     <t>A</t>
@@ -298,10 +298,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -309,6 +309,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -320,6 +328,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -335,36 +389,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -382,30 +406,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -414,14 +414,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -429,6 +422,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,7 +450,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -465,19 +465,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -489,7 +531,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,151 +621,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,17 +668,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -694,6 +688,21 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -717,7 +726,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -739,15 +748,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -759,7 +759,10 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -768,146 +771,143 @@
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1238,8 +1238,8 @@
   <sheetPr/>
   <dimension ref="A1:AT2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1559,36 +1559,36 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AD2">
       <formula1>"ACEH,BALI,BANTEN,BENGKULU,DAISTA YOGYAKARTA,DKI JAKARTA,JAMBI,JAWA BARAT,JAWA TENGAH,JAWA TIMUR,GORONTALO"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2">
+      <formula1>"Katolik,Kristen,Islam,Budha,Hindu,Lainnya"</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF2">
       <formula1>"SETIA BUDI,TEBET,MAMPANG PRAPATAN,PASAR MINGGU,KEBAYORAN LAMA,CILANDAK,KEBAYORAN BARU,PANCORAN,JAGAKARSA,PESANGGRAHAN"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AE2">
       <formula1>"KAB. ADM. KEP. SERIBU,KOTA ADM. JAKARTA PUSAT,KOTA ADM. JAKARTA UTARA,KOTA ADM. JAKARTA BARAT,KOTA ADM. JAKARTA SELATAN,KOTA ADM. JAKARTA TIMUR"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
-      <formula1>"Rekening Tabungan,Rekening Gaji,Transaksi Pribadi,Transaksi Bisnis,Lainnya"</formula1>
-    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AG2">
       <formula1>"RAJA WATI,KALIBATA,DUREN TIGA,CIKOKO,PENGADEGAN,PANCORAN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2">
+      <formula1>"Pegawai Swasta,Ibu Rumah Tangga,Lainnya"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AH2">
       <formula1>"Tidak Sekolah,SD,SMP,SMA,Diploma,S1 (Sarjana),S2 (Magister),S3 (Doktoral),Profesor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AK2">
-      <formula1>"Katolik,Kristen,Islam,Budha,Hindu,Lainnya"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AM2">
+      <formula1>"Rekening Tabungan,Rekening Gaji,Transaksi Pribadi,Transaksi Bisnis,Lainnya"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AN2">
       <formula1>"Gaji Bulanan,Pemasukan dari Usaha,Hasil Investasi,Warisan,Danah Hibah,Dana Pinjaman,Hadiah,Pendapatan Jasa,Pendapatan dari Keluarga (Suami/Istri/Orang Tua)"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AO2">
-      <formula1>"Pegawai Swasta,Ibu Rumah Tangga,Lainnya"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AP2">
       <formula1>"Jasa,Lainnya"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1" display="stgcrmf320@yopmail.com" tooltip="mailto:stgcrmf320@yopmail.com"/>
+    <hyperlink ref="K2" r:id="rId1" display="senyumku45622497@yopmail.com" tooltip="mailto:senyumku45622497@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>